<commit_message>
Add Employee entity and load_employees command
</commit_message>
<xml_diff>
--- a/data/targets.xlsx
+++ b/data/targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Takeda\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Projects\TakedaAnalitic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2493,7 +2493,7 @@
     <t>entity</t>
   </si>
   <si>
-    <t>employee</t>
+    <t>employee_name</t>
   </si>
 </sst>
 </file>
@@ -3479,8 +3479,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:H801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A781" workbookViewId="0">
-      <selection activeCell="B798" sqref="B798"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>